<commit_message>
updated data files, began writing functions
</commit_message>
<xml_diff>
--- a/tutorial/data/transport_model_v1/transport_model_data.xlsx
+++ b/tutorial/data/transport_model_v1/transport_model_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chunter\Documents\Projects\portfolio-analysis\tyche\tutorial\data\transport_model_v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63409FCC-122B-49EB-8039-90DEBBB50347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53484E-1944-4101-B7E9-7884B5140954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
+    <workbookView xWindow="-11175" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="154">
   <si>
     <t>Technology</t>
   </si>
@@ -496,6 +496,12 @@
   </si>
   <si>
     <t>transport_model</t>
+  </si>
+  <si>
+    <t>Energy consumption</t>
+  </si>
+  <si>
+    <t>Energy storage power</t>
   </si>
 </sst>
 </file>
@@ -851,7 +857,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D3" sqref="D3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,10 +1130,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED80D3D-A266-4C3A-9AD4-96FF102588A4}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1184,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <f>123500/E26</f>
+        <f>123500/E27</f>
         <v>82333.333333333328</v>
       </c>
       <c r="F2" t="s">
@@ -1632,7 +1638,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>153</v>
       </c>
       <c r="D20">
         <v>18</v>
@@ -1644,7 +1650,7 @@
         <v>48</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1655,7 +1661,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21">
         <v>19</v>
@@ -1664,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21" t="s">
         <v>78</v>
@@ -1678,19 +1684,19 @@
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <v>20</v>
       </c>
       <c r="E22">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1701,43 +1707,43 @@
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D23">
         <v>21</v>
       </c>
       <c r="E23">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24">
+        <v>22</v>
+      </c>
+      <c r="E24">
         <f>15*33*1.136</f>
         <v>562.31999999999994</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F24" t="s">
         <v>65</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24">
-        <v>22</v>
-      </c>
-      <c r="E24">
-        <v>0.15</v>
-      </c>
-      <c r="F24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G24" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1748,19 +1754,19 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="D25">
         <v>23</v>
       </c>
       <c r="E25">
-        <v>0.75</v>
+        <v>0.15</v>
       </c>
       <c r="F25" t="s">
         <v>58</v>
       </c>
       <c r="G25" t="s">
-        <v>136</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1771,19 +1777,19 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>135</v>
       </c>
       <c r="D26">
         <v>24</v>
       </c>
       <c r="E26">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1794,42 +1800,65 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D27">
         <v>25</v>
       </c>
       <c r="E27">
+        <v>1.5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28">
+        <v>26</v>
+      </c>
+      <c r="E28">
         <f>10180/1.136</f>
         <v>8961.2676056338041</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F28" t="s">
         <v>67</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
         <v>59</v>
       </c>
-      <c r="D28">
-        <v>26</v>
-      </c>
-      <c r="E28">
+      <c r="D29">
+        <v>27</v>
+      </c>
+      <c r="E29">
         <v>50</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>102</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1842,16 +1871,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF24522-E239-407E-9D5E-D7C144EC6ADB}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1945,6 +1974,20 @@
       </c>
       <c r="D6" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1955,10 +1998,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8D442E4-5D42-45B6-A9DF-27F70F744A60}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,6 +2240,20 @@
       </c>
       <c r="D14">
         <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated transport model data files and functions
</commit_message>
<xml_diff>
--- a/tutorial/data/transport_model_v1/transport_model_data.xlsx
+++ b/tutorial/data/transport_model_v1/transport_model_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chunter\Documents\Projects\portfolio-analysis\tyche\tutorial\data\transport_model_v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E53484E-1944-4101-B7E9-7884B5140954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A88AAD-6FAE-4743-B7EF-8E798A5EB0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11175" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="163">
   <si>
     <t>Technology</t>
   </si>
@@ -502,6 +502,33 @@
   </si>
   <si>
     <t>Energy storage power</t>
+  </si>
+  <si>
+    <t>Dwell time basis</t>
+  </si>
+  <si>
+    <t>Selection of fuel/energy storage for dwell time calculation (0 = fuel storage, 1 = battery)</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Inverse of diesel fuel economy of 7 mile/dge (duplicates design variable)</t>
+  </si>
+  <si>
+    <t>Dwell time boolean</t>
+  </si>
+  <si>
+    <t>Boolean to turn on or off dwell time costs (1 = on, 0 = off)</t>
+  </si>
+  <si>
+    <t>Carbon cost boolean</t>
+  </si>
+  <si>
+    <t>Boolean to turn on or off carbon costs (1 = on, 0 = off)</t>
+  </si>
+  <si>
+    <t>Input fuel efficiency</t>
   </si>
 </sst>
 </file>
@@ -857,13 +884,14 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D8"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1130,10 +1158,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED80D3D-A266-4C3A-9AD4-96FF102588A4}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <f>123500/E27</f>
+        <f>123500/E29</f>
         <v>82333.333333333328</v>
       </c>
       <c r="F2" t="s">
@@ -1754,19 +1782,19 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>154</v>
       </c>
       <c r="D25">
         <v>23</v>
       </c>
       <c r="E25">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1777,19 +1805,19 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="D26">
         <v>24</v>
       </c>
       <c r="E26">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>58</v>
+        <v>156</v>
       </c>
       <c r="G26" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1800,19 +1828,19 @@
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D27">
         <v>25</v>
       </c>
       <c r="E27">
-        <v>1.5</v>
+        <v>0.15</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1823,43 +1851,136 @@
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="D28">
         <v>26</v>
       </c>
       <c r="E28">
+        <v>0.75</v>
+      </c>
+      <c r="F28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>27</v>
+      </c>
+      <c r="E29">
+        <v>1.5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30">
+        <v>28</v>
+      </c>
+      <c r="E30">
         <f>10180/1.136</f>
         <v>8961.2676056338041</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F30" t="s">
         <v>67</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G30" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" t="s">
         <v>59</v>
       </c>
-      <c r="D29">
-        <v>27</v>
-      </c>
-      <c r="E29">
+      <c r="D31">
+        <v>29</v>
+      </c>
+      <c r="E31">
         <v>50</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F31" t="s">
         <v>102</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G31" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32">
+        <v>30</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>156</v>
+      </c>
+      <c r="G32" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33">
+        <v>31</v>
+      </c>
+      <c r="E33">
+        <f>1/(7*1.136)</f>
+        <v>0.12575452716297789</v>
+      </c>
+      <c r="F33" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1874,7 +1995,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,10 +2063,10 @@
         <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1956,10 +2077,10 @@
         <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1970,10 +2091,10 @@
         <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1984,10 +2105,10 @@
         <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2001,7 +2122,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,7 +2329,7 @@
         <v>126</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2222,7 +2343,7 @@
         <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2236,7 +2357,7 @@
         <v>126</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -2250,7 +2371,7 @@
         <v>126</v>
       </c>
       <c r="C15" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="D15">
         <v>4</v>

</xml_diff>

<commit_message>
updated transport model data and functions; works but lifetime parameter is not set properly; need to define cost for more intuitive calculations
</commit_message>
<xml_diff>
--- a/tutorial/data/transport_model_v1/transport_model_data.xlsx
+++ b/tutorial/data/transport_model_v1/transport_model_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chunter\Documents\Projects\portfolio-analysis\tyche\tutorial\data\transport_model_v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A88AAD-6FAE-4743-B7EF-8E798A5EB0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDDFA54-765F-4F7D-BCAF-4E5A640ABBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
+    <workbookView xWindow="15" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="167">
   <si>
     <t>Technology</t>
   </si>
@@ -529,6 +529,18 @@
   </si>
   <si>
     <t>Input fuel efficiency</t>
+  </si>
+  <si>
+    <t>Output efficiency</t>
+  </si>
+  <si>
+    <t>Output price</t>
+  </si>
+  <si>
+    <t>mile/mile</t>
+  </si>
+  <si>
+    <t>Placeholder varible since output is needed</t>
   </si>
 </sst>
 </file>
@@ -881,10 +893,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E0C2A8-672C-44C9-8C07-E73AD8FD7772}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,6 +1162,75 @@
         <v>54</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" t="s">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1161,13 +1242,13 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2122,7 +2203,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E10" sqref="A10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,42 +2466,42 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B047988B-C110-4617-A337-95A7DDC0A719}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="M1:P2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>116</v>
       </c>
-      <c r="N1" t="s">
+      <c r="B1" t="s">
         <v>117</v>
       </c>
-      <c r="O1" t="s">
+      <c r="C1" t="s">
         <v>118</v>
       </c>
-      <c r="P1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>119</v>
       </c>
-      <c r="N2" t="s">
+      <c r="B2" t="s">
         <v>120</v>
       </c>
-      <c r="O2" t="s">
+      <c r="C2" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed phase-1 model and data; now fully working
</commit_message>
<xml_diff>
--- a/tutorial/data/transport_model_v1/transport_model_data.xlsx
+++ b/tutorial/data/transport_model_v1/transport_model_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chunter\Documents\Projects\portfolio-analysis\tyche\tutorial\data\transport_model_v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDDFA54-765F-4F7D-BCAF-4E5A640ABBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABE7526-1EA3-4601-977B-D8109B87515D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
+    <workbookView xWindow="3540" yWindow="3960" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="171">
   <si>
     <t>Technology</t>
   </si>
@@ -541,6 +541,18 @@
   </si>
   <si>
     <t>Placeholder varible since output is needed</t>
+  </si>
+  <si>
+    <t>Tractor lifetime</t>
+  </si>
+  <si>
+    <t>Vehicle lifetime before being retired</t>
+  </si>
+  <si>
+    <t>mile/yr</t>
+  </si>
+  <si>
+    <t>Yearly vehicle miles travelled (scale)</t>
   </si>
 </sst>
 </file>
@@ -893,10 +905,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E0C2A8-672C-44C9-8C07-E73AD8FD7772}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1182,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1193,41 +1205,18 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>165</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>164</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" t="s">
         <v>166</v>
       </c>
     </row>
@@ -1239,10 +1228,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ED80D3D-A266-4C3A-9AD4-96FF102588A4}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,6 +2053,29 @@
         <v>157</v>
       </c>
     </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>167</v>
+      </c>
+      <c r="D34">
+        <v>32</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2073,10 +2085,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DF24522-E239-407E-9D5E-D7C144EC6ADB}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,16 +2119,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2124,16 +2136,16 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2144,11 +2156,14 @@
         <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
         <v>45</v>
       </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2158,10 +2173,10 @@
         <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2172,10 +2187,10 @@
         <v>126</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2186,9 +2201,23 @@
         <v>126</v>
       </c>
       <c r="C7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
         <v>133</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2203,7 +2232,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="A10:E10"/>
+      <selection activeCell="B11" sqref="B11:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
organized transport_model folders and updated ReadMe with more documenation
</commit_message>
<xml_diff>
--- a/tutorial/data/transport_model_v1/transport_model_data.xlsx
+++ b/tutorial/data/transport_model_v1/transport_model_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chunter\Documents\Projects\portfolio-analysis\tyche\tutorial\data\transport_model_v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABE7526-1EA3-4601-977B-D8109B87515D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46CDF6F-0848-4E11-BBE7-43B9B2E2AFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="3960" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
+    <workbookView xWindow="525" yWindow="-15810" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{D052CFEE-CC97-4BB4-A7CC-34ED2B2386ED}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -495,9 +495,6 @@
     <t>Baseline scenario</t>
   </si>
   <si>
-    <t>transport_model</t>
-  </si>
-  <si>
     <t>Energy consumption</t>
   </si>
   <si>
@@ -553,6 +550,9 @@
   </si>
   <si>
     <t>Yearly vehicle miles travelled (scale)</t>
+  </si>
+  <si>
+    <t>transport_model_v1</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1182,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -1191,10 +1191,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G12" t="s">
         <v>165</v>
-      </c>
-      <c r="G12" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,7 +1205,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -1217,7 +1217,7 @@
         <v>58</v>
       </c>
       <c r="G13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1736,7 +1736,7 @@
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D20">
         <v>18</v>
@@ -1852,7 +1852,7 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D25">
         <v>23</v>
@@ -1861,10 +1861,10 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1875,7 +1875,7 @@
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D26">
         <v>24</v>
@@ -1884,10 +1884,10 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D32">
         <v>30</v>
@@ -2023,10 +2023,10 @@
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2037,7 +2037,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D33">
         <v>31</v>
@@ -2050,7 +2050,7 @@
         <v>53</v>
       </c>
       <c r="G33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2061,7 +2061,7 @@
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D34">
         <v>32</v>
@@ -2073,7 +2073,7 @@
         <v>20</v>
       </c>
       <c r="G34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2087,7 +2087,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2125,10 +2125,10 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" t="s">
         <v>169</v>
-      </c>
-      <c r="E2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2201,7 +2201,7 @@
         <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D7" t="s">
         <v>52</v>
@@ -2467,7 +2467,7 @@
         <v>126</v>
       </c>
       <c r="C14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -2603,8 +2603,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,7 +2653,7 @@
         <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
         <v>112</v>

</xml_diff>